<commit_message>
D-18 Completed scrapping amazon using selenium
</commit_message>
<xml_diff>
--- a/amazon_smart watches.xlsx
+++ b/amazon_smart watches.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,39 +463,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Smart Watches for Men Women Android &amp; iPhone, 1.83'' Touch Screen Fitness Tracker Watch with Bluetooth Calls (Make/Answer), Health Monitor, IP68 Waterproof, 120 Sport Models, 14 Days Battery Life</t>
+          <t>Amazfit Bip 5 Smart Watch 46mm, GPS, Alexa Built-in, Bluetooth Calling, 10-Day Battery, Heart-Rate &amp; VO2 Max, Sleep Health Monitoring, AI Fitness App,120+ Sports Modes, for Android &amp; iPhone, White</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$49.99</t>
+          <t>$69.99</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4.2 out of 5 stars, rating details</t>
+          <t>4.1 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>315</t>
+          <t>1,772</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Display-Compatible-Android-Bluetooth-Waterproof/dp/B0CSYLNSQK/ref=sr_1_1?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-1</t>
+          <t>https://www.amazon.com/Amazfit-Bluetooth-Calling-Tracking-Monitoring/dp/B0C7VRZ4Q7/ref=sr_1_1?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Amazfit GTR Mini Smart Watch 43mm, 14-Day Battery Life, GPS, AI Fitness App Enabled, Heart Rate &amp; Sleep Health Monitoring, 120+ Sports Modes, 5 ATM Water Resistance, Android iPhone Compatible, Pink</t>
+          <t>Smart Watches for Men Women Android &amp; iPhone, 1.83'' Touch Screen Fitness Tracker Watch with Bluetooth Calls (Make/Answer), Health Monitor, IP68 Waterproof, 120 Sport Models, 14 Days Battery Life</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$69.99</t>
+          <t>$49.99</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,19 +505,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>885</t>
+          <t>315</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Amazfit-Satellite-Positioning-Monitoring-Resistance/dp/B0BWF2YS2N/ref=sr_1_2?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-2</t>
+          <t>https://www.amazon.com/Display-Compatible-Android-Bluetooth-Waterproof/dp/B0CSYLNSQK/ref=sr_1_2?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Amazfit Bip 5 Smart Watch 46mm, GPS, Alexa Built-in, Bluetooth Calling, 10-Day Battery, Heart-Rate &amp; VO2 Max, Sleep Health Monitoring, AI Fitness App,120+ Sports Modes, for Android &amp; iPhone, White</t>
+          <t>Amazfit GTR Mini Smart Watch 43mm, 14-Day Battery Life, GPS, AI Fitness App Enabled, Heart Rate &amp; Sleep Health Monitoring, 120+ Sports Modes, 5 ATM Water Resistance, Android iPhone Compatible, Pink</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -527,368 +527,2420 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.1 out of 5 stars, rating details</t>
+          <t>4.2 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1,778</t>
+          <t>887</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Amazfit-Bluetooth-Calling-Tracking-Monitoring/dp/B0C7VRZ4Q7/ref=sr_1_3?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-3</t>
+          <t>https://www.amazon.com/Amazfit-Satellite-Positioning-Monitoring-Resistance/dp/B0BWF2YS2N/ref=sr_1_3?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Smart Watch for Women Men for Android Phones iPhone Compatible, 2.09'' Smartwatches Fitness Tracker with Call/SMS/Heart Rate/Blood Oxygen Monitor/Pedometer/2 Bnads (Black)</t>
+          <t>Samsung Electronics Galaxy Watch 4 Classic 46mm Smartwatch with ECG Monitor Tracker for Health Fitness Running Sleep Cycles GPS Fall Detection Bluetooth US Version, Black (Renewed)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$39.97</t>
+          <t>$59.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5.0 out of 5 stars, rating details</t>
+          <t>4.3 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5,105</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/HCHLQL-Android-Compatible-Smartwatches-Pedometer/dp/B0DHRC74KS/ref=sr_1_4?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-4</t>
+          <t>https://www.amazon.com/Samsung-Electronics-Smartwatch-Detection-Bluetooth/dp/B09JKYS2MZ/ref=sr_1_4?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Google Pixel Watch 2 (Previous Model) with the Best of Fitbit - Heart Rate Tracking, Stress Management, Safety Features - Android Smartwatch - Matte Black Aluminum Case - Obsidian Active Band - WI-FI</t>
+          <t>Google Pixel Watch 1st Gen (Previous Model) - Android Smartwatch with Fitbit Activity Tracking - Heart Rate Tracking Watch - Matte Black Stainless Steel case with Obsidian Active band - WiFi</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$145.92</t>
+          <t>$86.71</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.2 out of 5 stars, rating details</t>
+          <t>4.1 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1,449</t>
+          <t>3,299</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Google-Pixel-Watch-Best-Fitbit/dp/B0CCQ7DNQL/ref=sr_1_5?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-5</t>
+          <t>https://www.amazon.com/Google-Pixel-Watch-Smartwatch-Stainless/dp/B0BDSGHVMW/ref=sr_1_5?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Fitbit Inspire 3 Health &amp;-Fitness-Tracker with Stress Management, Workout Intensity, Sleep Tracking, 24/7 Heart Rate and more, Midnight Zen/Black One Size (S &amp; L Bands Included)</t>
+          <t>Garmin vívoactive 5, Health and Fitness GPS Smartwatch, AMOLED Display, Up to 11 Days of Battery, Orchid</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$99.00</t>
+          <t>$245.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4.3 out of 5 stars, rating details</t>
+          <t>4.4 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>16,253</t>
+          <t>3,937</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Fitbit-Management-Intensity-Tracking-Midnight/dp/B0B5F9SZW7/ref=sr_1_6?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-6</t>
+          <t>https://www.amazon.com/Garmin-v%C3%ADvoactive-Fitness-Smartwatch-Display/dp/B0CG6LMQHH/ref=sr_1_6?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samsung Galaxy Watch 6 Classic 47mm Bluetooth Smartwatch, Rotating Bezel, Fitness Tracker, Personalized HR Zones, Advanced Sleep Coaching, Heart Monitor, BIA Sensor, Health Insights, US Version, Black</t>
+          <t>Garmin fēnix® 8 – 51 mm, AMOLED, Sapphire, Premium Multisport GPS Smartwatch, Long-Lasting Battery Life, Dive-Rated, Built-in LED Flashlight, Carbon Gray DLC Titanium with Pebble Gray Band</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$195.58</t>
+          <t>$999.99</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4.5 out of 5 stars, rating details</t>
+          <t>5.0 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7,078</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/SAMSUNG-Bluetooth-Smartwatch-Rotating-Personalized/dp/B0C79918S5/ref=sr_1_7?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-7</t>
+          <t>https://www.amazon.com/Garmin-f%C4%93nix%C2%AE-Multisport-Long-Lasting-Built/dp/B0DD5DTVRJ/ref=sr_1_7?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Garmin fēnix® 8 – 51 mm, AMOLED, Sapphire, Premium Multisport GPS Smartwatch, Long-Lasting Battery Life, Dive-Rated, Built-in LED Flashlight, Carbon Gray DLC Titanium with Pebble Gray Band</t>
+          <t>SAMSUNG Galaxy Watch 4 40mm Smartwatch with ECG Monitor Tracker for Health, Fitness, Running, Sleep Cycles, GPS Fall Detection, Bluetooth, US Version, SM-R860NZKAXAA, Black</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$999.99</t>
+          <t>$73.97</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5.0 out of 5 stars, rating details</t>
+          <t>4.6 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>29,290</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Garmin-f%C4%93nix%C2%AE-Multisport-Long-Lasting-Built/dp/B0DD5DTVRJ/ref=sr_1_8?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-8</t>
+          <t>https://www.amazon.com/Samsung-Electronics-Smartwatch-Detection-Bluetooth/dp/B096BJLZZM/ref=sr_1_8?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Garmin Instinct 2X Solar - Tactical Edition, Rugged GPS Smartwatch, Built-in Flashlight, Ballistics Calculator, Solar Charging Capability, Coyote Tan</t>
+          <t>Garmin Venu 3 Slate Stainless Steel Bezel 1.4-Inch AMOLED Touchscreen Display Smart Watch with 45mm Black Case and Silicone Band</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$359.00</t>
+          <t>$357.97</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>4.6 out of 5 stars, rating details</t>
+          <t>4.4 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>2,793</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Garmin-Instinct-Solar-Smartwatch-Built/dp/B0BW2VKGXX/ref=sr_1_9?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-9</t>
+          <t>https://www.amazon.com/Garmin-Stainless-1-4-Inch-Touchscreen-Silicone/dp/B0CDC6H66Y/ref=sr_1_9?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-9</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ladies Watch for Women, Large Screen Smartwatch Bluetooth with Answer/Make Call/Text, Waterproof Smart Watch for Android iOS Phones with Fitness Activity Tracker and Pedometer</t>
+          <t>ALKAI Smart Watch Rugged and Military with 5ATM Waterproof Bluetooth Call(Answer/Dial Calls) AI Assistant, Long-Lasting Battery Life, Multiple Sports Tracking, Health Monitoring, 2.02'' HD Display</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>$25.10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5.0 out of 5 stars, rating details</t>
+          <t>3.8 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>73</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Junywell-Watch-Women-Smart-Fitness/dp/B0DN5MZ893/ref=sr_1_10?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-10</t>
+          <t>https://www.amazon.com/ALKAI-Waterproof-Bluetooth-Long-Lasting-Monitoring/dp/B0CJ9GG4V7/ref=sr_1_10?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Garmin Venu 3 Slate Stainless Steel Bezel 1.4-Inch AMOLED Touchscreen Display Smart Watch with 45mm Black Case and Silicone Band</t>
+          <t>Garmin Instinct 2X Solar - Tactical Edition, Rugged GPS Smartwatch, Built-in Flashlight, Ballistics Calculator, Solar Charging Capability, Coyote Tan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$357.97</t>
+          <t>$336.93 delivery</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4.4 out of 5 stars, rating details</t>
+          <t>4.6 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2,788</t>
+          <t>304</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Garmin-Stainless-1-4-Inch-Touchscreen-Silicone/dp/B0CDC6H66Y/ref=sr_1_11?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-11</t>
+          <t>https://www.amazon.com/Garmin-Instinct-Solar-Smartwatch-Built/dp/B0BW2VKGXX/ref=sr_1_11?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-11</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ALKAI Smart Watch Rugged and Military with 5ATM Waterproof Bluetooth Call(Answer/Dial Calls) AI Assistant, Long-Lasting Battery Life, Multiple Sports Tracking, Health Monitoring, 2.02'' HD Display</t>
+          <t>Smart Watch for Women Men for Android Phones iPhone Compatible, 2.09'' Smartwatches Fitness Tracker with Call/SMS/Heart Rate/Blood Oxygen Monitor/Pedometer/2 Bnads (Black)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$25.10</t>
+          <t>$39.97</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3.8 out of 5 stars, rating details</t>
+          <t>5.0 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/ALKAI-Waterproof-Bluetooth-Long-Lasting-Monitoring/dp/B0CJ9GG4V7/ref=sr_1_13?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-13</t>
+          <t>https://www.amazon.com/HCHLQL-Android-Compatible-Smartwatches-Pedometer/dp/B0DHRC74KS/ref=sr_1_13?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-13</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SAMSUNG Galaxy Watch 4 40mm Smartwatch with ECG Monitor Tracker for Health, Fitness, Running, Sleep Cycles, GPS Fall Detection, Bluetooth, US Version, SM-R860NZDAXAA, Pink Gold</t>
+          <t>Fitbit Inspire 3 Health &amp;-Fitness-Tracker with Stress Management, Workout Intensity, Sleep Tracking, 24/7 Heart Rate and more, Midnight Zen/Black One Size (S &amp; L Bands Included)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$81.89</t>
+          <t>$96.99</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4.6 out of 5 stars, rating details</t>
+          <t>4.3 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>29,289</t>
+          <t>16,256</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Samsung-Galaxy-Watch-Smartwatch-Detection/dp/B096BK7W5M/ref=sr_1_14?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-14</t>
+          <t>https://www.amazon.com/Fitbit-Management-Intensity-Tracking-Midnight/dp/B0B5F9SZW7/ref=sr_1_14?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-14</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Google Pixel Watch - Android Smartwatch with Fitbit Activity Tracking - Heart Rate Tracking - Polished Silver Stainless Steel case with Chalk Active band - WiFi</t>
+          <t>Samsung Galaxy Watch 6 40mm LTE Smartwatch, Fitness Tracker, Personalized HR Zones, Advanced Sleep Coaching, Heart Monitor, BIA Sensor for Health Wellness Insights, Big Screen, US Version, Gold</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>$86.08</t>
+          <t>$161.61</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4.1 out of 5 stars, rating details</t>
+          <t>4.5 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3,299</t>
+          <t>7,077</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Google-Pixel-Watch-Smartwatch-Stainless/dp/B0BDSHFLMZ/ref=sr_1_15?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-15</t>
+          <t>https://www.amazon.com/SAMSUNG-Smartwatch-Personalized-Advanced-Coaching/dp/B0C78QRD92/ref=sr_1_15?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-15</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Smart Watch for Men Women, 1.81" Large Screen Smartwatch Bluetooth with Answer/Make Call/Text, Waterproof Smart Watch for Android iOS Phones</t>
+          <t>Apple Watch SE (2nd Gen) [GPS 40mm] Smartwatch with Starlight Aluminium Case with Starlight Sport Band S/M. Fitness and Sleep Trackers, Crash Detection, Heart Rate Monitor, Retina Display</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>$179.80</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5.0 out of 5 stars, rating details</t>
+          <t>4.5 out of 5 stars, rating details</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2,410</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.amazon.com/Junywell-Smart-Watch-Smartwatch-Waterproof/dp/B0DJ6PY5RL/ref=sr_1_16?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-16</t>
+          <t>https://www.amazon.com/Apple-Smartwatch-Starlight-Aluminium-Detection/dp/B0DGJ73CFS/ref=sr_1_16?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-16</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Apple Watch Series 10 [GPS 46mm case] Smartwatch with Jet Black Aluminium Case with Black Sport Band - M/L. Fitness Tracker, ECG App, Always-On Retina Display, Water Resistant</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>$362.05</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1,691</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Smartwatch-Aluminium-Always/dp/B0DGHQ2QH6/ref=sr_1_18?dib=eyJ2IjoiMSJ9.AWcfzxBOvQ-PCz-fh1ikyX7XqMh_0TKd440vKdCB2IRgZ4lOM_PyLiAnidT_FlVyqMaLADsYlO3cBwuwKy8YUcyZXcY6l-1-Nzbj7AtC0by2LMJFDCujb3xMmbB5sCkCMDOAEn0ouf7ctpPZwSBmKToMu8kjYJ6Xye3vSrcg4aC8kvjG5e028xAWNySXjJOBykbPJ7CLo6prcXHH6288jwvb9rMyj_XqtZfRiJtnPSM.rV5JNC4PdWY4RlEzt6vRPKyyHjDIVWV9MohRnlKaSxQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114605&amp;sr=8-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Fitbit Versa 4 Fitness Smartwatch with Daily Readiness, GPS, 24/7 Heart Rate, 40+ Exercise Modes, Sleep Tracking and more, Black/Graphite, One Size (S &amp; L Bands Included)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>$138.99</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>13,140</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Fitbit-Smartwatch-Readiness-Exercise-Tracking/dp/B0B4MWCFV4/ref=sr_1_17?dib=eyJ2IjoiMSJ9.H5CIs7KnXfMOpsT4BMN8yLOvF7Are3u8rBb63LItizkfmE8JrMSsKnDEycPi6JFORZiR8t6tS6ZunDELwvw4Hw.VfBz7jLCo5uyzCVfNrDcdS2QClkMJvGNMS4vFvJoDgM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114618&amp;sr=8-17&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Smart Watch, 1.91" Smartwatch for Men Women (Answer/Make Call), Fitness Tracker with 120+ Sport Modes, IP68 Waterproof, Heart Rate/Spo2/Sleep Monitor, Pedometer, Activity Tracker for Android iOS</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>5.0 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>124</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Smartwatch-Fitness-Waterproof-Pedometer-Activity/dp/B0DFGYBVDH/ref=sr_1_18?dib=eyJ2IjoiMSJ9.H5CIs7KnXfMOpsT4BMN8yLOvF7Are3u8rBb63LItizkfmE8JrMSsKnDEycPi6JFORZiR8t6tS6ZunDELwvw4Hw.VfBz7jLCo5uyzCVfNrDcdS2QClkMJvGNMS4vFvJoDgM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114618&amp;sr=8-18&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Garmin Venu® Sq 2 GPS Smartwatch, All-Day Health Monitoring, Long-Lasting Battery Life, AMOLED Display, Slate and Shadow Gray</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>$154.99</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1,284</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Smartwatch-All-Day-Monitoring-Long-Lasting/dp/B0B5VVNJBF/ref=sr_1_19?dib=eyJ2IjoiMSJ9.H5CIs7KnXfMOpsT4BMN8yLOvF7Are3u8rBb63LItizkfmE8JrMSsKnDEycPi6JFORZiR8t6tS6ZunDELwvw4Hw.VfBz7jLCo5uyzCVfNrDcdS2QClkMJvGNMS4vFvJoDgM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114618&amp;sr=8-19&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Smart Watch, 1.91"HD Smartwatch for Men Women (Answer/Make Call), 2025 Fitness Watch Heart Rate/Activity/Step/Sleep Monitor/SpO2, Step Counter IP68 Waterproof 110+ Sport Mode Watches for Android IOS</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>$50.00</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>5.0 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>245</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Smartwatch-Fitness-Activity-Monitor-Waterproof/dp/B0DFCQ1W4H/ref=sr_1_20?dib=eyJ2IjoiMSJ9.H5CIs7KnXfMOpsT4BMN8yLOvF7Are3u8rBb63LItizkfmE8JrMSsKnDEycPi6JFORZiR8t6tS6ZunDELwvw4Hw.VfBz7jLCo5uyzCVfNrDcdS2QClkMJvGNMS4vFvJoDgM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114618&amp;sr=8-20&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Apple Watch Ultra 2 [GPS + Cellular 49mm] Smartwatch, Sport Watch with Black Titanium Case with Black Trail Loop - M/L. Fitness Tracker, Precision GPS, Action Button, Carbon Neutral</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>$705.49</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1,146</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Cellular-Smartwatch-Titanium/dp/B0DGHYDYMR/ref=sr_1_21?dib=eyJ2IjoiMSJ9.H5CIs7KnXfMOpsT4BMN8yLOvF7Are3u8rBb63LItizkfmE8JrMSsKnDEycPi6JFOBZTmy0AqfjoJ7rIDnLlYKq1xY9ELIlTTSwI-0PYRxvn3ETPSH1sJHF1gSQuYzSd45P_l9cVObk6G-xiGtO4DDu3U0rGnr3lv1bgfOxZx9OStGYezaumHFj43MFrnfG-5oeUg5boKsgQJm2L3eD7MJiWo46l24achLouuNzLKQQk.e6yAc5Z8KGuRUV_Azyew-dsk0NrSHuBXvux8jEcATcQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114618&amp;sr=8-21&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy Watch 5 Pro 45mm Smartwatch with GPS, Heart Rate, Fitness Tracking - Titanium, Sapphire Glass, Improved Battery</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>$164.83</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2,718</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/SAMSUNG-Bluetooth-Smartwatch-Improved-Sapphire/dp/B0B2HXJZ98/ref=sr_1_33?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-33&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Apple Watch SE (2nd Gen) [GPS 40mm] Smartwatch with Starlight Aluminum Case with Starlight Sport Band S/M. Fitness &amp; Sleep Tracker, Crash Detection, Heart Rate Monitor</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$181.57</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>3,425</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Smartwatch-Starlight-Aluminum-Detection/dp/B0CHX7R6WJ/ref=sr_1_34?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-34&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Michael Kors Men's or Women's Gen 6 44mm Touchscreen Smart Watch with Alexa Built-In, Fitness Tracker, Sleep Tracker, GPS, Music Control, Smartphone Notifications (Model: MKT5134V)</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>$167.99</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1,424</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Michael-Touchscreen-Fitness-Smartphone-Notifications/dp/B09CWSZ4B6/ref=sr_1_35?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-35&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>Apple Watch Series 10 [GPS + Cellular 46mm case] Smartwatch with Slate Titanium Case with Slate Milanese Loop - M/L. Fitness Tracker, ECG App, Always-On Retina Display, Carbon Neutral</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>$721.71</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>4.7 out of 5 stars, rating details</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>406</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Titanium-Milanese/dp/B0DGHYDYNP/ref=sr_1_18?dib=eyJ2IjoiMSJ9.yku8xfj6b0X6JL8PmK6rmycRUHwy-2mgWiR7ei2BVTAsvCrNFBHeGgXOepkU-sVPo51kHG8PVtTsJjdhyhOx4ENi2-K_6HAQKgftAFK6iIQ7x2YrnmjorEir7pjXg0fYp2vtLGBzNED9X8_RoqiRHAruak9lbWpzpNzckLaqxjeWVU3JAciR4h5OBy2vVIHLM2jIRX03lols3ATxngCaos7a-JqdmZ_p8CTkLWEmN70.QVX6Aol3OzLlRVKYotqq-mb9qV156pzmBRnPSYnKUqw&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737043021&amp;sr=8-18</t>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Titanium-Milanese/dp/B0DGHYDYNP/ref=sr_1_36?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-36&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ALKAI Smart Watch Rugged and Military with 5ATM Waterproof Bluetooth Call(Answer/Dial Calls) AI Voice Assistant, Long-Lasting Battery Life, Multiple Sports Tracking, Health Monitoring</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$18.50</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>5.0 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/ALKAI-Waterproof-Bluetooth-Long-Lasting-Monitoring/dp/B0D6RMHTGC/ref=sr_1_37?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-37&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Amazfit Cheetah Smart Watch 47mm, Dual-band GPS, AI Fitness Running Coach, Alexa-Built In, 14 Day Battery Life, Fitness Watch with 150+ Sports Modes, Heart Rate Sleep Monitoring, for Android iPhone</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$124.99</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Amazfit-Cheetah-Alexa-Built-Workouts-Marathons/dp/B0C6TD76SN/ref=sr_1_38?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-38&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Garmin Lily 2, Small and Stylish Smartwatch, Hidden Display, Patterned Lens, Up to 5 Days Battery Life, Coconut</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$310.63</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>279</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Stylish-Smartwatch-Display-Patterned/dp/B0CP9C4RKN/ref=sr_1_39?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-39&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Garmin Instinct Crossover Solar, Rugged Hybrid Smartwatch with Solar Charging Capabilities, Analog Hands and Digital Display, Tidal Blue, Adjustable</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>$359.99</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Instinct-Crossover-Smartwatch-Capabilities/dp/B0BHTVXMMB/ref=sr_1_40?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-40&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Garmin epix Gen 2, Premium active smartwatch, Health and wellness features, touchscreen AMOLED display, adventure watch with advanced features, white titanium</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>$59.88 delivery</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-smartwatch-wellness-touchscreen-adventure/dp/B09NMLVQ64/ref=sr_1_41?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-41&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Garmin Enduro™ 3 – 51 mm, Solar, Sapphire, Ultraperformance GPS Smartwatch, Extreme Battery Life, Detailed Mapping, Built-in LED Flashlight, Carbon Gray DLC Titanium with Black UltraFit Nylon Strap</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>$799.99</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-EnduroTM-Ultraperformance-Smartwatch-Built/dp/B0DD5N9G17/ref=sr_1_42?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-42&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SAMSUNG Galaxy Watch 4 Classic 46mm Smartwatch with ECG Monitor Tracker for Health, Fitness, Running, Sleep Cycles, GPS Fall Detection &amp; Bluetooth, US Version, Black</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>$104.01</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>3,377</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Samsung-Electronics-Smartwatch-Detection-Bluetooth/dp/B096BKFG57/ref=sr_1_43?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-43&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Garmin Forerunner® 965 Running Smartwatch, Colorful AMOLED Display, Training Metrics and Recovery Insights, Whitestone and Powder Gray</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>$529.99</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>198</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Forerunner%C2%AE-Smartwatch-Colorful-Whitestone/dp/B0BS1TN8QL/ref=sr_1_44?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-44&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Citizen CZ Smart PQ2 Hybrid Smartwatch with YouQ Wellness app Featuring IBM Watson® AI and NASA Research, Black and White Customizable Display, Bluetooth, HR, Activity Tracker, 18-Day Battery Life</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>$178.45</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>288</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Citizen-Smartwatch-Featuring-Customizable-Bluetooth/dp/B0BZWGJC6Z/ref=sr_1_45?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-45&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Garmin Forerunner® 255 Music, GPS Running Smartwatch with Music, Advanced Insights, Long-Lasting Battery, Black - 010-02641-20</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>$249.99</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>1,157</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Forerunner%C2%AE-Smartwatch-Advanced-Long-Lasting/dp/B09WTV6MMY/ref=sr_1_46?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-46&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Garmin Forerunner 265 Running Smartwatch, Colorful AMOLED Display, Training Metrics and Recovery Insights, Black and Powder Gray</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>$414.99</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>524</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Forerunner-Smartwatch-Colorful-Training/dp/B0BS1T9J4Y/ref=sr_1_47?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-47&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Amazfit Active Edge Smart Watch 46 mm, Rugged Sport &amp; Fitness Watch, GPS, AI Health SCoach for Outdoor, Workouts &amp; Exercise, 16 Days Battery, 130+ Sports Modes, Android iPhone Compatible, Mint Green</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>$85.00</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>7,484</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Amazfit-Stylish-Workouts-Exercise-resistant/dp/B0CFY3ZSPZ/ref=sr_1_48?dib=eyJ2IjoiMSJ9.e6nzX0DeCWVGC5NLNPj2_UAatGHnA1Eet-fIuWOQh4aSn1dKtpFyF6mNm85l2w74abKzKNXlS2cdP-ouC_0eXI3sAboi1M3c-wvEqXsLHxaXVSHNcYGuU4wPo8YWHmn5bGqD3OOY-QbqUKPRM5X6ucRkKPyOPHrg9r7pp-fioFHS7r3pltT4fLWGVtfX5qiKmRxrnBglqLWJONj8USPJXFKvjMxOSqXqqcBOkUfRMKs.JweJGb2U1K1A3ednmYX2XaNR96B_-4mIaCSYhmaT63U&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114620&amp;sr=8-48&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 8 [GPS + Cellular, 45mm] - Midnight Aluminum Case with Midnight Sport Band, M/L (Renewed)</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>768</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-GPS-Cellular-45mm/dp/B0BNFGKSNF/ref=sr_1_50?dib=eyJ2IjoiMSJ9.p4FaZR6HF88rTLmwPsOdJi0SvlFtqNrUEnAtFWHrRZU6WIUWClQselCLuxugSRSt.0hRU1EJXQUVFpQYEV1RILdpdsg7T1jRfd-idhw91jXc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114623&amp;sr=8-50&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Garmin vivoactive 4S, Smaller-Sized GPS Smartwatch, Features Music, Body Energy Monitoring, Animated Workouts, Pulse Ox Sensors and More, Silver with Gray Band</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>$279.95</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>17,176</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-v%C3%ADvoactive-Smaller-Sized-Smartwatch-Monitoring/dp/B07W7W9DQQ/ref=sr_1_51?dib=eyJ2IjoiMSJ9.p4FaZR6HF88rTLmwPsOdJi0SvlFtqNrUEnAtFWHrRZU6WIUWClQselCLuxugSRSt.0hRU1EJXQUVFpQYEV1RILdpdsg7T1jRfd-idhw91jXc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114623&amp;sr=8-51&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Garmin Instinct 3 AMOLED 50mm (Neo Tropic/Twilight) Rugged Outdoor GPS Smartwatch Bundle - Metal Bezel, Built-in Flashlight, Long Battery Life with PlayBetter Portable Charger &amp; HD Screen Protectors</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Instinct-Twilight-Outdoor-Smartwatch/dp/B0DSCFF231/ref=sr_1_52?dib=eyJ2IjoiMSJ9.p4FaZR6HF88rTLmwPsOdJi0SvlFtqNrUEnAtFWHrRZU6WIUWClQselCLuxugSRSt.0hRU1EJXQUVFpQYEV1RILdpdsg7T1jRfd-idhw91jXc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114623&amp;sr=8-52&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 9 [GPS 41mm] Smartwatch with Pink Aluminum Case with Light Pink Sport Band S/M. Fitness Tracker, ECG Apps, Always-On Retina Display, Water Resistant (MR933LW/A)</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>$379.99</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>8,365</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Smartwatch-Aluminum-Fitness-Resistant/dp/B0CSV9Y331/ref=sr_1_53?dib=eyJ2IjoiMSJ9.p4FaZR6HF88rTLmwPsOdJi0SvlFtqNrUEnAtFWHrRZU6WIUWClQselCLuxugSRSt.0hRU1EJXQUVFpQYEV1RILdpdsg7T1jRfd-idhw91jXc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114623&amp;sr=8-53&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Smart Watch for Men Fitness Watch Wireless Smart Bracelet 116Plus Phone Fitness Watch for Women Waterproof Blood Pressure Test for Men Women Red.</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>$7.95</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Hbbgdiy-Wireless-Bracelet-Waterproof-Pressure/dp/B0DGLM35N8/ref=sr_1_65?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-65&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Military Smart Watches for Men with LED Flashlight, Tactical Rugged Smart Watch with 1.45" HD, 3ATM Waterproof &amp; Compass, Sports Fitness Tracker with Heart rate/SPO2/Sleep Monitor</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>$39.00</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Leuceira-Military-Flashlight-Tactical-Waterproof/dp/B0D9GZ4BC3/ref=sr_1_66?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-66&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Military Smart Watches for Men Make Call 1.39" HD Big Screen Fitness Tracker Rugged Tactical Smartwatch Compatible with iPhone Samsung Android Phones Heart Rate Sleep Monitor Sports Watch</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>$54.99</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>4.1 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Military-Watches-Tactical-Smartwatch-Compatible/dp/B0BK4Q1P9C/ref=sr_1_67?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-67&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 8 (GPS, 45mm) Midnight Aluminum Case with Midnight Sport Band (Renewed Premium)</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>365</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Midnight-Aluminum-Renewed/dp/B0C2VT692T/ref=sr_1_68?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-68&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 7 (GPS + Cellular, 41mm) Midnight Aluminum Case with Midnight Sport Band, Regular (Renewed)</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>661</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Cellular-Midnight-Aluminum/dp/B09PB1PTH8/ref=sr_1_69?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-69&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Garmin vivomove Sport, Hybrid Smartwatch, Health and Wellness Features, Touchscreen, Light Green</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>$146.71</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>3.9 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1,352</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-vivomove-Smartwatch-Wellness-Touchscreen/dp/B09LRKTYZB/ref=sr_1_70?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-70&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Smart Watch for Samsung Galaxy S23 FE - with Bluetooth Call, 1.9" HD Touch Screen Fitness Tracker 50+ Sport Modes Elegant Activity Tracker for Android/iOS Phones - Black</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>$34.99</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>5.0 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Smart-Watch-Samsung-Galaxy-S23/dp/B0DCCC63HY/ref=sr_1_71?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-71&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Fitbit Versa Lite Edition Smart Watch,GPS, One Size (S and L Bands Included)</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>$79.99</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>5,006</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Fitbit-Versa-Smart-Watch-included/dp/B07MFZ9MHM/ref=sr_1_72?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-72&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Motorola Moto Watch 70 - Health and Fitness Smartwatch for Every Day Wear, Advanced Health Features, Up to 10 Days Battery Life - Compatible with Android and iOS, Phantom Black</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>$72.00</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>3.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>167</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Motorola-Moto-Watch-Smartwatch-Compatible/dp/B0C234ML6S/ref=sr_1_73?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-73&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Smart Watch for Men Women, 1.83" HD Fitness Tracker with Answer/Make Calls, Heart Rate/Blood Oxygen/Sleep Monitor, Pedometer, Calories, 120+ Sports Mode, IP68 Waterproof Fitness Watch for Android iOS</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>$5.10 delivery</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>268</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Fitness-Tracker-Pedometer-Calories-Waterproof/dp/B0DKBT3YP8/ref=sr_1_74?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-74&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Motorola Moto 40 Smartwatch -10 Days Battery Life, Google Fit Integration, 1.5'' Crystal Clear Display, Heart Tracking, in-Depth Sleep Tracking, iOS and Android Compatible - Rose Gold</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>$62.41</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>3.5 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Motorola-Smartwatch-Integration-Tracking-Compatible/dp/B0CRDX9TF6/ref=sr_1_75?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-75&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 8 [GPS 41mm] Smart Watch w/Midnight Aluminum Case with Midnight Sport Band - S/M. Fitness Tracker, Blood Oxygen &amp; ECG Apps, Always-On Retina Display, Water Resistant</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>23,372</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Midnight-Aluminum-Always/dp/B0BDJBG74R/ref=sr_1_76?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-76&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Smart Watch for Samsung Galaxy S24 S24+ Ultra - with Bluetooth Call, 1.9" HD Touch Screen Fitness Tracker 50+ Sport Modes Elegant Activity Tracker for Android/iOS Phones - Black</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>$34.99</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Smart-Watch-Samsung-Galaxy-Ultra/dp/B0DCC8VQ8H/ref=sr_1_77?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-77&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Apple Watch SE (2nd Gen) [GPS 40mm] Smart Watch w/Starlight Aluminum Case &amp; Starlight Sport Band - S/M. Fitness &amp; Sleep Tracker, Crash Detection, Heart Rate Monitor, Retina Display, Water Resistant</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>3,068</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Smart-Starlight-Aluminum/dp/B0BDHTQDRZ/ref=sr_1_78?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-78&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 9 [GPS + Cellular, 41mm] - Gold Stainless Steel Case with Gold Sport Band, S/M (Renewed)</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>4.8 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Stainless-Fitness/dp/B0CTD7MBPH/ref=sr_1_79?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-79&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Garmin tactix® 7 – AMOLED Edition, Specialized Military and Tactical GPS Smartwatch, Adaptive AMOLED Display, Built-in Flashlight, Preloaded TopoActive Mapping</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>$1,329.99</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-tactix%C2%AE-Specialized-Smartwatch-Built/dp/B0CGJXT7RB/ref=sr_1_80?dib=eyJ2IjoiMSJ9.tVlh-4-fJhT4fXyH1KKVq0snE4ibtQD9GZBmWMhpnczeAuafaVE0qcpZ5d4EHArGN_1GBcvjVXP0UFZhlYILM-qxVOawrn0BllcF_U-z9GhYURA-MHxgfQG5X2AE_yHLW2qkJbghTg7KSTWwH_mVayhxnxOuv5cBLqZbbdb6wBAQqYfqo-8kGpsjLy1IzpMqPNnricYQzL_gm3w1yw80i1vtGDRc0coxB44j0pST-iY.yiQ4eoBZMCviT7pqEd62eVN6-7t4R0zJ7NwQ4CFXbFE&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114625&amp;sr=8-80&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>iTouch Sport 4 Smartwatch - Fitness Tracker, Heart Rate Monitor, Customizable Watch Face - Activity and Calorie Tracker - 100+ Sports Modes - Bluetooth Connectivity</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>$39.99</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>3.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/iTouch-Sport-Smartwatch-Customizable-Connectivity/dp/B0CHL2JJMG/ref=sr_1_81?dib=eyJ2IjoiMSJ9.AyGMMyiFF8H72MyzMWbyNqMGcKoxa9haZAWZjuY80dv4gOUy5ypUViYZR9t8tFD3TVTkgxcNlVCJg7TS3yxyoQ.Qz6WCvyA8QgaaBVebKiYNyvGAcNxGvLvM8Gbj9jXZTM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114628&amp;sr=8-81&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy Watch4 44MM SM-R870 Aluminum Smartwatch GPS Only (Renewed)</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>$73.98</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>1,135</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/SAMSUNG-Smartwatch-Monitor-Detection-Bluetooth/dp/B09CSXXXPG/ref=sr_1_82?dib=eyJ2IjoiMSJ9.AyGMMyiFF8H72MyzMWbyNqMGcKoxa9haZAWZjuY80dv4gOUy5ypUViYZR9t8tFD3TVTkgxcNlVCJg7TS3yxyoQ.Qz6WCvyA8QgaaBVebKiYNyvGAcNxGvLvM8Gbj9jXZTM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114628&amp;sr=8-82&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy Watch Active2 Bluetooth Smartwatch, Aluminum, 44mm, Black (SM-R820NZKCXAR) (Renewed)</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2,052</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Samsung-Galaxy-Active-Smartwatch-Charging/dp/B081KB2FJ2/ref=sr_1_83?dib=eyJ2IjoiMSJ9.AyGMMyiFF8H72MyzMWbyNqMGcKoxa9haZAWZjuY80dv4gOUy5ypUViYZR9t8tFD3TVTkgxcNlVCJg7TS3yxyoQ.Qz6WCvyA8QgaaBVebKiYNyvGAcNxGvLvM8Gbj9jXZTM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114628&amp;sr=8-83&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 5 (GPS + Cellular, 40MM) - Space Gray Aluminum Case with Black Sport Band (Renewed)</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>27,611</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-GPS-Cellular-40MM/dp/B0843HV4D5/ref=sr_1_84?dib=eyJ2IjoiMSJ9.AyGMMyiFF8H72MyzMWbyNqMGcKoxa9haZAWZjuY80dv4gOUy5ypUViYZR9t8tFD3TVTkgxcNlVCJg7TS3yxyoQ.Qz6WCvyA8QgaaBVebKiYNyvGAcNxGvLvM8Gbj9jXZTM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114628&amp;sr=8-84&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Apple Watch Ultra 2 [GPS + Cellular 49mm] Smartwatch with Rugged Titanium Case &amp; Blue Ocean Band. Fitness Tracker, Precision GPS, Action Button, Extra-Long Battery Life, Bright Retina Display</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>1,568</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Precision-Extra-Long/dp/B0CHWZ5VVM/ref=sr_1_85?dib=eyJ2IjoiMSJ9.AyGMMyiFF8H72MyzMWbyNqMGcKoxa9haZAWZjuY80dv4gOUy5ypUViYZR9t8tFD3TVTkgxcNlVCJg7TS3yxyoQ.Qz6WCvyA8QgaaBVebKiYNyvGAcNxGvLvM8Gbj9jXZTM&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114628&amp;sr=8-85&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Huawei Watch 2 Sport Smartwatch - Ceramic Bezel - Carbon Black Strap (US Warranty)</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>4.0 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>1,102</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Huawei-Watch-Sport-Smartwatch-Warranty/dp/B06XDMCH6Z/ref=sr_1_97?dib=eyJ2IjoiMSJ9.BGXPBuyAAGNzDB6uzyFCVMRihK85x7wzksR2P1EVDqFqm8uN6UMH99ngY9WwODpzq7nuvNa2X9VfNG8Km16YKQ.sLccN6rb12rqmFTvnyXsAeT77k-Qa9xRMT0njqwCGZQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114630&amp;sr=8-97&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Citizen CZ Smart PQ2 41MM Unisex Smartwatch with YouQ App with IBM Watson® AI and NASA research, Wear OS by Google, HR, GPS, Fitness Tracker, Amazon Alexa™, iPhone Android Compatible, IPX6 Rating</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>$175.00</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>3.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Citizen-Smartwatch-Featuring-Research-Touchscreen/dp/B0BR8JS8L9/ref=sr_1_98?dib=eyJ2IjoiMSJ9.BGXPBuyAAGNzDB6uzyFCVMRihK85x7wzksR2P1EVDqFqm8uN6UMH99ngY9WwODpzq7nuvNa2X9VfNG8Km16YKQ.sLccN6rb12rqmFTvnyXsAeT77k-Qa9xRMT0njqwCGZQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114630&amp;sr=8-98&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 6 (GPS, 44mm) - Blue Aluminum Case with Deep Navy Sport Band (Renewed)</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>9,985</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/New-Apple-Watch-GPS-44mm/dp/B08KTW1YD3/ref=sr_1_99?dib=eyJ2IjoiMSJ9.BGXPBuyAAGNzDB6uzyFCVMRihK85x7wzksR2P1EVDqFqm8uN6UMH99ngY9WwODpzq7nuvNa2X9VfNG8Km16YKQ.sLccN6rb12rqmFTvnyXsAeT77k-Qa9xRMT0njqwCGZQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114630&amp;sr=8-99&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Garmin 010-02173-11 Venu, GPS Smartwatch with Bright Touchscreen Display, Features Music, Body Energy Monitoring, Animated Workouts, Pulse Ox Sensor and More, Black</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>$229.95</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>7,275</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Garmin-Smartwatch-Touchscreen-Monitoring-010-02173-11/dp/B07WLN9RYD/ref=sr_1_100?dib=eyJ2IjoiMSJ9.BGXPBuyAAGNzDB6uzyFCVMRihK85x7wzksR2P1EVDqFqm8uN6UMH99ngY9WwODpzq7nuvNa2X9VfNG8Km16YKQ.sLccN6rb12rqmFTvnyXsAeT77k-Qa9xRMT0njqwCGZQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114630&amp;sr=8-100&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>aeac Smart Watch for Men Women, 2024 Newest Fitness Watch (2-Pack) - White+Green</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>$59.99</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/aeac-Smart-Newest-Fitness-2-Pack/dp/B0DJS982DT/ref=sr_1_101?dib=eyJ2IjoiMSJ9.BGXPBuyAAGNzDB6uzyFCVMRihK85x7wzksR2P1EVDqFqm8uN6UMH99ngY9WwODpzq7nuvNa2X9VfNG8Km16YKQ.sLccN6rb12rqmFTvnyXsAeT77k-Qa9xRMT0njqwCGZQ&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114630&amp;sr=8-101&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy Watch 2019 (46mm) Bluetooth, Wi-Fi, GPS Smartwatch, SM-R800 - International Version (Silver)</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2,295</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Samsung-Galaxy-Bluetooth-Smartwatch-SM-R800/dp/B07P5JSCMZ/ref=sr_1_113?dib=eyJ2IjoiMSJ9.9-rMgei4l3QkUKtwLA6mP7OTWGX4RCyIlIJwguDRDFA-aKaLhKHv0RQY_7vbq7QE8eFFbWdBXIQNe38qW8092Q.IP187cYDvE1NJe-b0SIpqMsK5Xvj1sFnoe7jRCMc26E&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114632&amp;sr=8-113&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Smart Watches for Men Women, Fitness Watch with Heart Rate/SpO2/Sleep Monitor, Pedometer, IP68 Waterproof for iPhone Android</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>$69.80</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Watches-Fitness-Monitor-Pedometer-Waterproof/dp/B0CN96XV5Y/ref=sr_1_114?dib=eyJ2IjoiMSJ9.9-rMgei4l3QkUKtwLA6mP7OTWGX4RCyIlIJwguDRDFA-aKaLhKHv0RQY_7vbq7QE8eFFbWdBXIQNe38qW8092Q.IP187cYDvE1NJe-b0SIpqMsK5Xvj1sFnoe7jRCMc26E&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114632&amp;sr=8-114&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Accutime Kids Love, Diana Show Educational Learning Touchscreen Pink Smart Watch Toy with Graphic Strap for Girls, Boys, Toddlers - Selfie Cam, Games, Alarm, Calculator, Pedometer (Model: LDA4037AZ)</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>$28.87</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Accutime-Educational-Learning-Touchscreen-Toddlers/dp/B0B46V6CMW/ref=sr_1_115?dib=eyJ2IjoiMSJ9.9-rMgei4l3QkUKtwLA6mP7OTWGX4RCyIlIJwguDRDFA-aKaLhKHv0RQY_7vbq7QE8eFFbWdBXIQNe38qW8092Q.IP187cYDvE1NJe-b0SIpqMsK5Xvj1sFnoe7jRCMc26E&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114632&amp;sr=8-115&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Apple Watch SE (GPS + Cellular, 40mm) - Silver Aluminum Case with White Sport Band (Renewed)</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>$123.97</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>458</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/New-Apple-Watch-Cellular-40mm/dp/B08KJ3LJBX/ref=sr_1_116?dib=eyJ2IjoiMSJ9.9-rMgei4l3QkUKtwLA6mP7OTWGX4RCyIlIJwguDRDFA-aKaLhKHv0RQY_7vbq7QE8eFFbWdBXIQNe38qW8092Q.IP187cYDvE1NJe-b0SIpqMsK5Xvj1sFnoe7jRCMc26E&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114632&amp;sr=8-116&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 9 [GPS + Cellular 41mm] Smartwatch with Silver Aluminum Case with Storm Blue Sport Band S/M. Fitness Tracker, Blood Oxygen &amp; ECG Apps, Always-On Retina Display</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Aluminum-Fitness/dp/B0CHX9X566/ref=sr_1_117?dib=eyJ2IjoiMSJ9.9-rMgei4l3QkUKtwLA6mP7OTWGX4RCyIlIJwguDRDFA-aKaLhKHv0RQY_7vbq7QE8eFFbWdBXIQNe38qW8092Q.IP187cYDvE1NJe-b0SIpqMsK5Xvj1sFnoe7jRCMc26E&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114632&amp;sr=8-117&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Bundle of Amazfit Bip 5 Smartwatch (Pink) + 22mm Nylon Replacement Band (Grey)</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>$95.92</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Bundle-Amazfit-Smartwatch-Nylon-Replacement/dp/B0D7D6M4V7/ref=sr_1_130?dib=eyJ2IjoiMSJ9.lS66EYFhfU7oYGDiejquSqOvN4sITK4-tO0v0PuHrNLjFtDZyYZPBFJ745jp1KnO.CaOO7Jo4UHlMlwCxrl--szgxfgNh3VWdm4jruF62YVc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114634&amp;sr=8-130&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 9 [GPS + Cellular 41mm] Smartwatch with Midnight Aluminum Case with Midnight Sport Band S/M. Fitness Tracker, Blood Oxygen &amp; ECG Apps, Always-On Retina Display</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Cellular-Smartwatch-Midnight-Aluminum/dp/B0CHXB6CNY/ref=sr_1_131?dib=eyJ2IjoiMSJ9.lS66EYFhfU7oYGDiejquSqOvN4sITK4-tO0v0PuHrNLjFtDZyYZPBFJ745jp1KnO.CaOO7Jo4UHlMlwCxrl--szgxfgNh3VWdm4jruF62YVc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114634&amp;sr=8-131&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Samsung Gear Sport Smartwatch (Bluetooth), Blue, SM-R600NZBAXAR – US Version with Warranty</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>$190.97</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>540</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Samsung-Sport-Smartwatch-Bluetooth-SM-R600NZBAXAR/dp/B075X4RQHZ/ref=sr_1_132?dib=eyJ2IjoiMSJ9.lS66EYFhfU7oYGDiejquSqOvN4sITK4-tO0v0PuHrNLjFtDZyYZPBFJ745jp1KnO.CaOO7Jo4UHlMlwCxrl--szgxfgNh3VWdm4jruF62YVc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114634&amp;sr=8-132&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Accutime Kids Disney Minnie Mouse Multicolor Educational Learning Touchscreen Smart Watch Toy for Girls, Boys, Toddlers - Selfie Cam, Learning Games, Alarm, Calculator and More (Model: MN4325AZ)</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>$29.60</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>4.1 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Accutime-Disney-Minnie-Interactive-smartwatch/dp/B09XGXJ9NN/ref=sr_1_133?dib=eyJ2IjoiMSJ9.lS66EYFhfU7oYGDiejquSqOvN4sITK4-tO0v0PuHrNLjFtDZyYZPBFJ745jp1KnO.CaOO7Jo4UHlMlwCxrl--szgxfgNh3VWdm4jruF62YVc&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114634&amp;sr=8-133&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Military Smart Watch for Men 800mAh Big Battery Smartwatch with 1.85” Screen Rugged Smartwatch 100+ Sports Modes Fitness Tracker with Heart Rate/SpO2/Sleep Monitor Answer Call for iPhone Android</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>$59.99</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Military-Battery-Smartwatch-Fitness-Tracker/dp/B0DQX7SF5T/ref=sr_1_147?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-147&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Smart Watches for Men Women, Fitness Watch with Heart Rate/SpO2/Sleep Monitor, Pedometer, IP68 Waterproof for iPhone Android</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>$79.95</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Watches-Fitness-Monitor-Pedometer-Waterproof/dp/B0CN97S374/ref=sr_1_148?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-148&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Military Smart Watches for Men with LED Flashlight Rugged Smartwatch with 730mAh Big Battery 1.85”Big Screen Tactical Fitness Tracker Heart Rate Sleep Monitor Make/Answer Calls for iPhone Android</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>$59.99</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Military-Watches-Flashlight-Smartwatch-Tactical/dp/B0DP2CBGCH/ref=sr_1_149?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-149&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Samsung Gear S2 Smartwatch - Dark Gray</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>$149.25</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>4.2 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>3,138</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Samsung-Gear-S2-Smartwatch-Dark/dp/B015JQ62RY/ref=sr_1_150?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-150&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 9 [GPS, 41mm] - (PRODUCT)RED Aluminum Case with (PRODUCT)RED Sport Band, S/M (Renewed)</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>325</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-Product-Aluminum-Renewed/dp/B0CTDB3PZN/ref=sr_1_151?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-151&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Military Smart Watch for Men with LED Flashlight 400mAh Big Battery Outdoor Tactical Smartwatch with 3ATM Waterproof (Make/Answer Calls) Fitness Tracker with Heart Rate Sleep Monitor for iOS Android</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>$39.99</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Military-Flashlight-Tactical-Smartwatch-Waterproof/dp/B0DQTFYWVW/ref=sr_1_152?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-152&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Rival Smart Watches for Men, Women and Teens | All-in-One Fitness Watch, Ulti Charger 4 Ports with Quick Charger Boltz Pro Lightning Fast Charger Fast Charging Block for Smart Phones</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>$58.99</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/FREEZE2TRIM-Watches-Fitness-Lightning-Charging/dp/B0DS3TLX8Z/ref=sr_1_153?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-153&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Smart Watch 1.44inch Touch Screen Fitness Watch Waterproof Heart Rate Sports Pedometer Black</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>$25.99 delivery</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/MOUNTTU-1-44inch-Fitness-Waterproof-Pedometer/dp/B0DSC3J5WS/ref=sr_1_154?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-154&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Apple Watch SE (GPS + Cellular, 40mm) - Silver Aluminum Case with White Sport Band (Renewed)</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-SE-Cellular-40mm/dp/B08SWP54FH/ref=sr_1_155?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-155&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Military Smart Watch for Men with LED Flashlight 1.85” Big Screen Rugged Smart Watch 730mAh Large Battery 114 Sports Modes Fitness Watch Heart Rate Sleep Tracker Tactical Smartwatch for iOS Android</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>$75.99</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Military-Flashlight-Battery-Tactical-Smartwatch/dp/B0DP8DBPN6/ref=sr_1_156?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-156&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Bundle of Amazfit T-Rex 3 (Lava) Rugged/Military Smart Watch 48mm, GPS (with Privacy), Offline Maps,Black + Amazfit Up OWS Bluetooth 5.3 Headphones, Open Ear Wireless Earbuds with Easy Touch Control</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>$279.98</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Amazfit-T-Rex-Military-Bluetooth-Headphones/dp/B0DNTZT1FF/ref=sr_1_157?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-157&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>aeac Smart Watch for Men Women, 2024 Newest Fitness Watch (3-Pack) - Pink+Blue+Green</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>$110.00</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/aeac-Smart-Newest-Fitness-3-Pack/dp/B0DMVBHRR4/ref=sr_1_158?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-158&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>aeac Smart Watch for Women, Alexa Built-in, Stable Bluetooth Call, Fitness Tracker with Heart Rate/SpO2/Stress/Sleep Monitor, 100 Sports, IP68 Waterproof Smartwatches for iOS Android</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>$69.99</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/aeac-Bluetooth-Fitness-Waterproof-Smartwatches/dp/B0DQWY9LMB/ref=sr_1_159?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-159&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Apple Watch Series 8 [GPS + Cellular, 45mm] - Silver Aluminum Case with White Sport Band, M/L (Renewed)</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>$204.59</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars, rating details</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/Apple-Watch-GPS-Cellular-45MM/dp/B0BVTLLMH6/ref=sr_1_160?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-160&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>aeac Smart Watch for Men Women, 2024 Newest Fitness Watch (3-Pack) - Pink+Black+Green</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>$110.00</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/aeac-Smart-Newest-Fitness-3-Pack/dp/B0DMVC8GZJ/ref=sr_1_161?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-161&amp;xpid=WdCFZcJCteozA</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>aeac Smart Watch for Men Women, 2024 Newest Fitness Watch (3-Pack) - Black+Pink+White</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>$120.00</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/aeac-Smart-Newest-Fitness-3-Pack/dp/B0DMVCZSD7/ref=sr_1_162?dib=eyJ2IjoiMSJ9.k-pBYE3aiJdtde9_oTmorqv-kcQOLsZjPsqI1y8FWXKSEuwsbmOkpNP9A-XxwKK5J_dUdrSHSwZ4p1OOhC5PtMF5tE7gL0Er10cyd_DaQ_rpPJ_Bpz7Yo3nzXZ0pjGyt9wR24mX_wgrHZU_ao6hJg_XelQXOtJX032fgaa12bzM-2_ZO7RBzJieAeJOtd6ydALgl1V3GFYhbJVtk0nY7em2Yv9cvU9sMuvxlcbb22NA.QJogpRlsLL7d2iFxSGfIWo-ctPC75scNxx1xNEXfZ1c&amp;dib_tag=se&amp;keywords=smart+watches&amp;qid=1737114636&amp;sr=8-162&amp;xpid=WdCFZcJCteozA</t>
         </is>
       </c>
     </row>

</xml_diff>